<commit_message>
upload data dictionary, database ERD, database table creation SQL scripts
</commit_message>
<xml_diff>
--- a/Data_Dictionary.xlsx
+++ b/Data_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iGuest\Desktop\563\final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianxinsong/Documents/Tianxin/On-Campus/20spring/imt563/imt563_final_project_new/IMT563_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AD87AA-8691-4721-B81E-3D8B1BCE81CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEACF71-9B7C-F54C-8EDF-0955817761BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{2744FEC9-E11D-4AD5-AEAF-A0CA2BFA0122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2744FEC9-E11D-4AD5-AEAF-A0CA2BFA0122}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,62 +33,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>User</t>
   </si>
   <si>
-    <t>UserID(PK),  HistoryID(FK), WatchlistID(FK), FirstName, LastName, DOB, EmailID, PhoneNo, Password(encrypted)</t>
-  </si>
-  <si>
     <t>Movies</t>
   </si>
   <si>
-    <t>MovieID (PK), Title, Description, GenreID(FK), LanguageID(FK), IMDBRating, RTRating</t>
-  </si>
-  <si>
-    <t>TV Shows</t>
-  </si>
-  <si>
-    <t>TVShowID(PK), Title, Description, GenreID(FK), LanguageID(FK), Number of Seasons, Number of Episodes, IMDBRating, RTRating </t>
-  </si>
-  <si>
     <t>UserWatchHistory</t>
   </si>
   <si>
-    <t>HistoryID(PK), UserID(FK), MovieID, TVShowID, Date</t>
-  </si>
-  <si>
     <t>MovieStreamingPlatform</t>
   </si>
   <si>
-    <t>MSPID(PK), SPName, MovieID(FK)</t>
-  </si>
-  <si>
-    <t>TVShowStreamingPlatform</t>
-  </si>
-  <si>
-    <t>TVSPID(PK), SPName, TVShowID(FK)</t>
-  </si>
-  <si>
     <t>UserWatchList</t>
   </si>
   <si>
-    <t>UWLID(PK), UserID(FK), WatchlistID(FK), WatchlistName, MovieID (FK), TVShowID (FK)</t>
-  </si>
-  <si>
     <t>MovieReview</t>
   </si>
   <si>
-    <t>MovieID(PK,FK), MovieReviewID (PK), ReviewDesc</t>
-  </si>
-  <si>
-    <t>TVShowReview</t>
-  </si>
-  <si>
-    <t>TVShowID(PK,FK), TVShowReviewID(PK), ReviewDesc</t>
-  </si>
-  <si>
     <t>Genre</t>
   </si>
   <si>
@@ -101,29 +65,56 @@
     <t>LanguageID(PK), LanguageABBR, LanguageName</t>
   </si>
   <si>
-    <t>UserPreference</t>
-  </si>
-  <si>
-    <t>UserPreferenceID(PK), UserID(FK), LanguageID(FK), GenreID(FK)</t>
-  </si>
-  <si>
     <t>Data Dictionary</t>
   </si>
   <si>
     <t>Movie_Genre</t>
   </si>
   <si>
-    <t>TVShow_Genre</t>
-  </si>
-  <si>
     <t>StreamingPlatform</t>
+  </si>
+  <si>
+    <t>UserID(PK),  FirstName, LastName, DOB, EmailID, PhoneNo, Password(encrypted)</t>
+  </si>
+  <si>
+    <t>HistoryID(PK), UserID(FK), MovieID, Date</t>
+  </si>
+  <si>
+    <t>UWLID(PK), UserID(FK), WatchlistName, MovieID (FK)</t>
+  </si>
+  <si>
+    <t>UserPreferenceGenre</t>
+  </si>
+  <si>
+    <t>UserID(FK), GenreID(FK)</t>
+  </si>
+  <si>
+    <t>UserPreferenceLanguage</t>
+  </si>
+  <si>
+    <t>UserID(FK), LanguageID(FK)</t>
+  </si>
+  <si>
+    <t>MovieID(FK), GenreID(FK)</t>
+  </si>
+  <si>
+    <t>MovieID (PK), GenreID(FK), LanguageID(FK), Title, Description, IMDBRating, RTRating</t>
+  </si>
+  <si>
+    <t>MovieReviewID (PK), MovieID(FK), ReviewDesc</t>
+  </si>
+  <si>
+    <t>MSPID(PK), SPID(FK), MovieID(FK)</t>
+  </si>
+  <si>
+    <t>SPID(PK), SPName, SPAddress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,22 +128,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -175,23 +168,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,190 +504,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40D6491-7354-43A1-AEE0-F560B7A7DD7B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.9296875" customWidth="1"/>
-    <col min="3" max="3" width="43.796875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="9" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="3">
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C13">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>